<commit_message>
load calculation load due to current longitudinal load buoyancy temperature and shrinkage
moment calculation remains
</commit_message>
<xml_diff>
--- a/outputs/Live_Loads_Seismic.xlsx
+++ b/outputs/Live_Loads_Seismic.xlsx
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>240.2016</v>
+        <v>240.2015999999999</v>
       </c>
       <c r="D2" t="n">
         <v>454.5144000000001</v>
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>508.7832000000002</v>
+        <v>508.7832000000001</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -561,7 +561,7 @@
         <v>50.74</v>
       </c>
       <c r="F5" t="n">
-        <v>508.7832000000002</v>
+        <v>508.7832000000001</v>
       </c>
     </row>
     <row r="6">

</xml_diff>